<commit_message>
extractions of mutliple word doc CVs completed
</commit_message>
<xml_diff>
--- a/Output/Output.xlsx
+++ b/Output/Output.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\Ray\Ray PC Home\Raymond\Raymond Loh Wee Ping Resume\Race Academy\2021\Course Notes\RPA Projects\RPAJ01_JobMatchingForPlacements\Output\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{333512C4-D71D-4C2B-8CAC-70A0DB45D127}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C6CDD2B-2E22-460A-B17C-D890D21E9F30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3845" yWindow="380" windowWidth="6595" windowHeight="9330" xr2:uid="{2638BDFF-89C8-442F-9D0F-4A68B5387AE3}"/>
+    <workbookView xWindow="7055" yWindow="635" windowWidth="6595" windowHeight="9330" xr2:uid="{2638BDFF-89C8-442F-9D0F-4A68B5387AE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>